<commit_message>
May 2021 data update
</commit_message>
<xml_diff>
--- a/data/Wiesbaden First Pass Acceptance.xlsx
+++ b/data/Wiesbaden First Pass Acceptance.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2506966-B26C-4BC9-B8BF-5D6B5A84BED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4F2868-C043-4F1C-9128-809F7B28812B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5835" yWindow="165" windowWidth="18000" windowHeight="12735" activeTab="1" xr2:uid="{203EF309-F09C-46D6-B42C-975B3263EA61}"/>
+    <workbookView xWindow="19824" yWindow="-4344" windowWidth="34560" windowHeight="18744" activeTab="1" xr2:uid="{203EF309-F09C-46D6-B42C-975B3263EA61}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
     <sheet name="FPA" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FPA!$A$1:$J$1710</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FPA!$A$1:$J$1775</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11345" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11633" uniqueCount="799">
   <si>
     <t>SQA</t>
   </si>
@@ -2411,6 +2411,27 @@
   </si>
   <si>
     <t>Release 101</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Release 1.2</t>
+  </si>
+  <si>
+    <t>WI_C 34</t>
+  </si>
+  <si>
+    <t>Phase 3</t>
+  </si>
+  <si>
+    <t>WI_C 36</t>
+  </si>
+  <si>
+    <t>WI_C 37</t>
+  </si>
+  <si>
+    <t>WI_L27</t>
   </si>
 </sst>
 </file>
@@ -3281,22 +3302,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D811D2-7FE2-4400-8864-3E57D05FCB66}">
-  <dimension ref="A1:J1730"/>
+  <dimension ref="A1:J1775"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1716" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1731" sqref="H1731"/>
+      <pane ySplit="1" topLeftCell="A1733" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1775" sqref="I1775"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="47.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="12" style="4" customWidth="1"/>
     <col min="9" max="9" width="32" customWidth="1"/>
     <col min="10" max="10" width="72.140625" bestFit="1" customWidth="1"/>
@@ -47630,10 +47651,10 @@
         <v>757</v>
       </c>
       <c r="D1603" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E1603" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1603" s="5" t="s">
         <v>23</v>
@@ -47642,7 +47663,7 @@
         <v>31</v>
       </c>
       <c r="H1603" s="4">
-        <v>44313</v>
+        <v>44320</v>
       </c>
     </row>
     <row r="1604" spans="1:9" x14ac:dyDescent="0.25">
@@ -48065,32 +48086,29 @@
       </c>
     </row>
     <row r="1620" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1620" t="s">
+      <c r="A1620" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1620" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="C1620" t="s">
-        <v>314</v>
+        <v>665</v>
+      </c>
+      <c r="C1620" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="D1620" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1620">
-        <v>1</v>
-      </c>
-      <c r="F1620" s="5" t="s">
-        <v>767</v>
+        <v>62</v>
+      </c>
+      <c r="E1620" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1620" t="s">
+        <v>756</v>
       </c>
       <c r="G1620" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1620" s="4">
-        <v>44315</v>
-      </c>
-      <c r="I1620" t="s">
-        <v>15</v>
+        <v>44314</v>
       </c>
     </row>
     <row r="1621" spans="1:9" x14ac:dyDescent="0.25">
@@ -48104,20 +48122,23 @@
         <v>314</v>
       </c>
       <c r="D1621" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="E1621">
         <v>1</v>
       </c>
-      <c r="F1621" s="7" t="s">
-        <v>704</v>
+      <c r="F1621" s="5" t="s">
+        <v>767</v>
       </c>
       <c r="G1621" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1621" s="4">
         <v>44315</v>
       </c>
+      <c r="I1621" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="1622" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1622" t="s">
@@ -48136,7 +48157,7 @@
         <v>1</v>
       </c>
       <c r="F1622" s="7" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="G1622" t="s">
         <v>31</v>
@@ -48162,7 +48183,7 @@
         <v>1</v>
       </c>
       <c r="F1623" s="7" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G1623" t="s">
         <v>31</v>
@@ -48188,7 +48209,7 @@
         <v>1</v>
       </c>
       <c r="F1624" s="7" t="s">
-        <v>769</v>
+        <v>706</v>
       </c>
       <c r="G1624" t="s">
         <v>31</v>
@@ -48214,7 +48235,7 @@
         <v>1</v>
       </c>
       <c r="F1625" s="7" t="s">
-        <v>707</v>
+        <v>769</v>
       </c>
       <c r="G1625" t="s">
         <v>31</v>
@@ -48240,7 +48261,7 @@
         <v>1</v>
       </c>
       <c r="F1626" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G1626" t="s">
         <v>31</v>
@@ -48266,7 +48287,7 @@
         <v>1</v>
       </c>
       <c r="F1627" s="7" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G1627" t="s">
         <v>31</v>
@@ -48292,7 +48313,7 @@
         <v>1</v>
       </c>
       <c r="F1628" s="7" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G1628" t="s">
         <v>31</v>
@@ -48318,7 +48339,7 @@
         <v>1</v>
       </c>
       <c r="F1629" s="7" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G1629" t="s">
         <v>31</v>
@@ -48344,7 +48365,7 @@
         <v>1</v>
       </c>
       <c r="F1630" s="7" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G1630" t="s">
         <v>31</v>
@@ -48370,7 +48391,7 @@
         <v>1</v>
       </c>
       <c r="F1631" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G1631" t="s">
         <v>31</v>
@@ -48396,7 +48417,7 @@
         <v>1</v>
       </c>
       <c r="F1632" s="7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G1632" t="s">
         <v>31</v>
@@ -48422,7 +48443,7 @@
         <v>1</v>
       </c>
       <c r="F1633" s="7" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G1633" t="s">
         <v>31</v>
@@ -48448,7 +48469,7 @@
         <v>1</v>
       </c>
       <c r="F1634" s="7" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G1634" t="s">
         <v>31</v>
@@ -48474,17 +48495,14 @@
         <v>1</v>
       </c>
       <c r="F1635" s="7" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G1635" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1635" s="4">
         <v>44315</v>
       </c>
-      <c r="I1635" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="1636" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1636" t="s">
@@ -48503,14 +48521,17 @@
         <v>1</v>
       </c>
       <c r="F1636" s="7" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="G1636" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1636" s="4">
         <v>44315</v>
       </c>
+      <c r="I1636" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="1637" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1637" t="s">
@@ -48529,36 +48550,33 @@
         <v>1</v>
       </c>
       <c r="F1637" s="7" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G1637" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1637" s="4">
         <v>44315</v>
       </c>
-      <c r="I1637" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="1638" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1638" s="5" t="s">
+      <c r="A1638" t="s">
         <v>2</v>
       </c>
       <c r="B1638" s="5" t="s">
-        <v>665</v>
-      </c>
-      <c r="C1638" s="5" t="s">
-        <v>85</v>
+        <v>315</v>
+      </c>
+      <c r="C1638" t="s">
+        <v>314</v>
       </c>
       <c r="D1638" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1638" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1638" s="5" t="s">
-        <v>766</v>
+        <v>60</v>
+      </c>
+      <c r="E1638">
+        <v>1</v>
+      </c>
+      <c r="F1638" s="7" t="s">
+        <v>719</v>
       </c>
       <c r="G1638" t="s">
         <v>30</v>
@@ -48604,51 +48622,54 @@
         <v>2</v>
       </c>
       <c r="B1640" s="5" t="s">
-        <v>600</v>
+        <v>665</v>
       </c>
       <c r="C1640" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D1640" t="s">
-        <v>669</v>
+        <v>56</v>
       </c>
       <c r="E1640" s="5">
         <v>1</v>
       </c>
       <c r="F1640" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="G1640" s="5" t="s">
-        <v>29</v>
+        <v>766</v>
+      </c>
+      <c r="G1640" t="s">
+        <v>30</v>
       </c>
       <c r="H1640" s="4">
         <v>44315</v>
       </c>
+      <c r="I1640" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="1641" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1641" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1641" s="5" t="s">
-        <v>665</v>
+        <v>600</v>
       </c>
       <c r="C1641" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D1641" t="s">
-        <v>62</v>
+        <v>669</v>
       </c>
       <c r="E1641" s="5">
         <v>1</v>
       </c>
-      <c r="F1641" t="s">
-        <v>756</v>
-      </c>
-      <c r="G1641" t="s">
-        <v>31</v>
+      <c r="F1641" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="G1641" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="H1641" s="4">
-        <v>44314</v>
+        <v>44315</v>
       </c>
     </row>
     <row r="1642" spans="1:9" x14ac:dyDescent="0.25">
@@ -48942,28 +48963,28 @@
     </row>
     <row r="1653" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1653" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1653" s="5" t="s">
-        <v>315</v>
+        <v>1</v>
+      </c>
+      <c r="B1653" t="s">
+        <v>772</v>
       </c>
       <c r="C1653" t="s">
-        <v>314</v>
+        <v>442</v>
       </c>
       <c r="D1653" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="E1653">
-        <v>2</v>
-      </c>
-      <c r="F1653" s="7" t="s">
-        <v>704</v>
+        <v>1</v>
+      </c>
+      <c r="F1653" t="s">
+        <v>477</v>
       </c>
       <c r="G1653" t="s">
         <v>31</v>
       </c>
       <c r="H1653" s="4">
-        <v>44319</v>
+        <v>44316</v>
       </c>
     </row>
     <row r="1654" spans="1:9" x14ac:dyDescent="0.25">
@@ -48977,13 +48998,13 @@
         <v>314</v>
       </c>
       <c r="D1654" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E1654">
-        <v>2</v>
-      </c>
-      <c r="F1654" s="7" t="s">
-        <v>707</v>
+        <v>1</v>
+      </c>
+      <c r="F1654" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G1654" t="s">
         <v>31</v>
@@ -49003,13 +49024,13 @@
         <v>314</v>
       </c>
       <c r="D1655" t="s">
-        <v>59</v>
+        <v>301</v>
       </c>
       <c r="E1655">
-        <v>2</v>
-      </c>
-      <c r="F1655" s="7" t="s">
-        <v>708</v>
+        <v>1</v>
+      </c>
+      <c r="F1655" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G1655" t="s">
         <v>31</v>
@@ -49035,7 +49056,7 @@
         <v>2</v>
       </c>
       <c r="F1656" s="7" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="G1656" t="s">
         <v>31</v>
@@ -49061,7 +49082,7 @@
         <v>2</v>
       </c>
       <c r="F1657" s="7" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="G1657" t="s">
         <v>31</v>
@@ -49087,7 +49108,7 @@
         <v>2</v>
       </c>
       <c r="F1658" s="7" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="G1658" t="s">
         <v>31</v>
@@ -49113,7 +49134,7 @@
         <v>2</v>
       </c>
       <c r="F1659" s="7" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="G1659" t="s">
         <v>31</v>
@@ -49139,17 +49160,14 @@
         <v>2</v>
       </c>
       <c r="F1660" s="7" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="G1660" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1660" s="4">
         <v>44319</v>
       </c>
-      <c r="I1660" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="1661" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1661" t="s">
@@ -49165,13 +49183,13 @@
         <v>59</v>
       </c>
       <c r="E1661">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1661" s="7" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="G1661" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H1661" s="4">
         <v>44319</v>
@@ -49194,7 +49212,7 @@
         <v>2</v>
       </c>
       <c r="F1662" s="7" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
       <c r="G1662" t="s">
         <v>31</v>
@@ -49220,14 +49238,17 @@
         <v>2</v>
       </c>
       <c r="F1663" s="7" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="G1663" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1663" s="4">
         <v>44319</v>
       </c>
+      <c r="I1663" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="1664" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1664" t="s">
@@ -49243,13 +49264,13 @@
         <v>59</v>
       </c>
       <c r="E1664">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1664" s="7" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="G1664" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1664" s="4">
         <v>44319</v>
@@ -49266,13 +49287,13 @@
         <v>314</v>
       </c>
       <c r="D1665" t="s">
-        <v>301</v>
+        <v>59</v>
       </c>
       <c r="E1665">
-        <v>1</v>
-      </c>
-      <c r="F1665" s="5" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="F1665" s="7" t="s">
+        <v>718</v>
       </c>
       <c r="G1665" t="s">
         <v>31</v>
@@ -49292,13 +49313,13 @@
         <v>314</v>
       </c>
       <c r="D1666" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E1666">
-        <v>1</v>
-      </c>
-      <c r="F1666" s="5" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="F1666" s="7" t="s">
+        <v>717</v>
       </c>
       <c r="G1666" t="s">
         <v>31</v>
@@ -49308,25 +49329,25 @@
       </c>
     </row>
     <row r="1667" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1667" s="5" t="s">
+      <c r="A1667" t="s">
         <v>2</v>
       </c>
       <c r="B1667" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="C1667" s="5" t="s">
-        <v>85</v>
+        <v>315</v>
+      </c>
+      <c r="C1667" t="s">
+        <v>314</v>
       </c>
       <c r="D1667" t="s">
-        <v>666</v>
-      </c>
-      <c r="E1667" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1667" s="5" t="s">
-        <v>755</v>
-      </c>
-      <c r="G1667" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1667">
+        <v>2</v>
+      </c>
+      <c r="F1667" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="G1667" t="s">
         <v>31</v>
       </c>
       <c r="H1667" s="4">
@@ -49338,22 +49359,22 @@
         <v>2</v>
       </c>
       <c r="B1668" s="5" t="s">
-        <v>665</v>
+        <v>581</v>
       </c>
       <c r="C1668" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D1668" t="s">
-        <v>63</v>
+        <v>666</v>
       </c>
       <c r="E1668" s="5">
         <v>1</v>
       </c>
       <c r="F1668" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1668" t="s">
-        <v>29</v>
+        <v>755</v>
+      </c>
+      <c r="G1668" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="H1668" s="4">
         <v>44319</v>
@@ -49396,7 +49417,7 @@
         <v>85</v>
       </c>
       <c r="D1670" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E1670" s="5">
         <v>1</v>
@@ -49405,10 +49426,10 @@
         <v>23</v>
       </c>
       <c r="G1670" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1670" s="4">
-        <v>44321</v>
+        <v>44319</v>
       </c>
     </row>
     <row r="1671" spans="1:9" x14ac:dyDescent="0.25">
@@ -49416,13 +49437,13 @@
         <v>2</v>
       </c>
       <c r="B1671" s="5" t="s">
-        <v>665</v>
+        <v>765</v>
       </c>
       <c r="C1671" s="5" t="s">
-        <v>85</v>
+        <v>757</v>
       </c>
       <c r="D1671" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="E1671" s="5">
         <v>1</v>
@@ -49434,7 +49455,7 @@
         <v>31</v>
       </c>
       <c r="H1671" s="4">
-        <v>44321</v>
+        <v>44320</v>
       </c>
     </row>
     <row r="1672" spans="1:9" x14ac:dyDescent="0.25">
@@ -49442,25 +49463,28 @@
         <v>2</v>
       </c>
       <c r="B1672" s="5" t="s">
-        <v>559</v>
+        <v>765</v>
       </c>
       <c r="C1672" s="5" t="s">
-        <v>558</v>
-      </c>
-      <c r="D1672" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1672" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1672" s="7" t="s">
-        <v>779</v>
+        <v>757</v>
+      </c>
+      <c r="D1672" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1672" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1672" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G1672" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1672" s="4">
-        <v>44320</v>
+        <v>44327</v>
+      </c>
+      <c r="I1672" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="1673" spans="1:9" x14ac:dyDescent="0.25">
@@ -49474,19 +49498,22 @@
         <v>757</v>
       </c>
       <c r="D1673" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1673" s="5">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="E1673" s="8" t="s">
+        <v>254</v>
       </c>
       <c r="F1673" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G1673" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1673" s="4">
-        <v>44320</v>
+        <v>44327</v>
+      </c>
+      <c r="I1673" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="1674" spans="1:9" x14ac:dyDescent="0.25">
@@ -49500,19 +49527,19 @@
         <v>757</v>
       </c>
       <c r="D1674" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1674" s="5">
         <v>1</v>
       </c>
       <c r="F1674" s="5" t="s">
-        <v>780</v>
+        <v>23</v>
       </c>
       <c r="G1674" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1674" s="4">
-        <v>44320</v>
+        <v>44328</v>
       </c>
     </row>
     <row r="1675" spans="1:9" x14ac:dyDescent="0.25">
@@ -49526,13 +49553,13 @@
         <v>757</v>
       </c>
       <c r="D1675" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E1675" s="5">
         <v>1</v>
       </c>
       <c r="F1675" s="5" t="s">
-        <v>781</v>
+        <v>23</v>
       </c>
       <c r="G1675" t="s">
         <v>31</v>
@@ -49552,7 +49579,7 @@
         <v>757</v>
       </c>
       <c r="D1676" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E1676" s="5">
         <v>1</v>
@@ -49561,10 +49588,13 @@
         <v>23</v>
       </c>
       <c r="G1676" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1676" s="4">
-        <v>44320</v>
+        <v>44344</v>
+      </c>
+      <c r="I1676" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="1677" spans="1:9" x14ac:dyDescent="0.25">
@@ -49572,19 +49602,19 @@
         <v>2</v>
       </c>
       <c r="B1677" s="5" t="s">
-        <v>765</v>
+        <v>559</v>
       </c>
       <c r="C1677" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="D1677" t="s">
+        <v>558</v>
+      </c>
+      <c r="D1677" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E1677" s="5">
         <v>1</v>
       </c>
-      <c r="F1677" s="5" t="s">
-        <v>782</v>
+      <c r="F1677" s="7" t="s">
+        <v>779</v>
       </c>
       <c r="G1677" t="s">
         <v>31</v>
@@ -49598,21 +49628,21 @@
         <v>2</v>
       </c>
       <c r="B1678" s="5" t="s">
-        <v>765</v>
+        <v>749</v>
       </c>
       <c r="C1678" s="5" t="s">
-        <v>757</v>
+        <v>85</v>
       </c>
       <c r="D1678" t="s">
-        <v>7</v>
+        <v>667</v>
       </c>
       <c r="E1678" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1678" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1678" t="s">
+        <v>783</v>
+      </c>
+      <c r="G1678" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H1678" s="4">
@@ -49624,25 +49654,25 @@
         <v>2</v>
       </c>
       <c r="B1679" s="5" t="s">
-        <v>749</v>
+        <v>665</v>
       </c>
       <c r="C1679" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D1679" t="s">
-        <v>667</v>
+        <v>65</v>
       </c>
       <c r="E1679" s="5">
         <v>1</v>
       </c>
       <c r="F1679" s="5" t="s">
-        <v>783</v>
-      </c>
-      <c r="G1679" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1679" t="s">
         <v>31</v>
       </c>
       <c r="H1679" s="4">
-        <v>44320</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="1680" spans="1:9" x14ac:dyDescent="0.25">
@@ -49650,13 +49680,13 @@
         <v>2</v>
       </c>
       <c r="B1680" s="5" t="s">
-        <v>765</v>
+        <v>665</v>
       </c>
       <c r="C1680" s="5" t="s">
-        <v>757</v>
+        <v>85</v>
       </c>
       <c r="D1680" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="E1680" s="5">
         <v>1</v>
@@ -49665,146 +49695,140 @@
         <v>23</v>
       </c>
       <c r="G1680" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1680" s="4">
-        <v>44322</v>
-      </c>
-      <c r="I1680" t="s">
-        <v>15</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="1681" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1681" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1681" s="5" t="s">
-        <v>649</v>
+      <c r="A1681" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1681" t="s">
+        <v>772</v>
       </c>
       <c r="C1681" t="s">
-        <v>784</v>
+        <v>442</v>
       </c>
       <c r="D1681" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1681" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1681" s="5" t="s">
-        <v>23</v>
+        <v>59</v>
+      </c>
+      <c r="E1681">
+        <v>1</v>
+      </c>
+      <c r="F1681" t="s">
+        <v>792</v>
       </c>
       <c r="G1681" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1681" s="4">
-        <v>44322</v>
-      </c>
-      <c r="I1681" t="s">
-        <v>15</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="1682" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1682" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1682" s="5" t="s">
-        <v>749</v>
-      </c>
-      <c r="C1682" s="5" t="s">
-        <v>85</v>
+      <c r="A1682" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1682" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1682" t="s">
+        <v>442</v>
       </c>
       <c r="D1682" t="s">
-        <v>666</v>
-      </c>
-      <c r="E1682" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1682" s="5" t="s">
-        <v>783</v>
-      </c>
-      <c r="G1682" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1682">
+        <v>1</v>
+      </c>
+      <c r="F1682" t="s">
+        <v>477</v>
+      </c>
+      <c r="G1682" t="s">
         <v>31</v>
       </c>
       <c r="H1682" s="4">
-        <v>44326</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="1683" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1683" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1683" s="5" t="s">
-        <v>765</v>
-      </c>
-      <c r="C1683" s="5" t="s">
-        <v>757</v>
+      <c r="A1683" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1683" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1683" t="s">
+        <v>442</v>
       </c>
       <c r="D1683" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1683" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1683" s="5" t="s">
-        <v>23</v>
+        <v>59</v>
+      </c>
+      <c r="E1683">
+        <v>1</v>
+      </c>
+      <c r="F1683" t="s">
+        <v>775</v>
       </c>
       <c r="G1683" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H1683" s="4">
-        <v>44326</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="1684" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1684" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1684" s="5" t="s">
-        <v>649</v>
+      <c r="A1684" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1684" t="s">
+        <v>772</v>
       </c>
       <c r="C1684" t="s">
-        <v>784</v>
+        <v>442</v>
       </c>
       <c r="D1684" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1684" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1684" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="E1684">
+        <v>1</v>
+      </c>
+      <c r="F1684" t="s">
+        <v>775</v>
       </c>
       <c r="G1684" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H1684" s="4">
-        <v>44326</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="1685" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1685" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1685" s="5" t="s">
-        <v>665</v>
-      </c>
-      <c r="C1685" s="5" t="s">
-        <v>85</v>
+      <c r="A1685" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1685" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1685" t="s">
+        <v>442</v>
       </c>
       <c r="D1685" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1685" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1685" s="5" t="s">
-        <v>785</v>
-      </c>
-      <c r="G1685" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1685">
+        <v>1</v>
+      </c>
+      <c r="F1685" t="s">
+        <v>477</v>
+      </c>
+      <c r="G1685" t="s">
         <v>31</v>
       </c>
       <c r="H1685" s="4">
-        <v>44326</v>
+        <v>44321</v>
       </c>
     </row>
     <row r="1686" spans="1:9" x14ac:dyDescent="0.25">
@@ -49812,13 +49836,13 @@
         <v>2</v>
       </c>
       <c r="B1686" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="C1686" t="s">
-        <v>784</v>
+        <v>765</v>
+      </c>
+      <c r="C1686" s="5" t="s">
+        <v>757</v>
       </c>
       <c r="D1686" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E1686" s="5">
         <v>1</v>
@@ -49827,88 +49851,97 @@
         <v>23</v>
       </c>
       <c r="G1686" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1686" s="4">
-        <v>44323</v>
+        <v>44344</v>
       </c>
     </row>
     <row r="1687" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1687" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1687" s="5" t="s">
-        <v>649</v>
+      <c r="A1687" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1687" t="s">
+        <v>793</v>
       </c>
       <c r="C1687" t="s">
-        <v>784</v>
+        <v>268</v>
       </c>
       <c r="D1687" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1687" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1687" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1687">
+        <v>1</v>
+      </c>
+      <c r="F1687" t="s">
         <v>23</v>
       </c>
       <c r="G1687" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1687" s="4">
-        <v>44326</v>
+        <v>44322</v>
+      </c>
+      <c r="I1687" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1688" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1688" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1688" s="5" t="s">
-        <v>624</v>
+        <v>1</v>
+      </c>
+      <c r="B1688" t="s">
+        <v>793</v>
       </c>
       <c r="C1688" t="s">
-        <v>625</v>
+        <v>268</v>
       </c>
       <c r="D1688" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E1688">
         <v>1</v>
       </c>
-      <c r="F1688" s="7" t="s">
+      <c r="F1688" t="s">
         <v>23</v>
       </c>
       <c r="G1688" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1688" s="4">
-        <v>44323</v>
+        <v>44322</v>
+      </c>
+      <c r="I1688" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="1689" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1689" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1689" s="5" t="s">
-        <v>612</v>
+      <c r="A1689" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1689" t="s">
+        <v>793</v>
       </c>
       <c r="C1689" t="s">
-        <v>611</v>
+        <v>268</v>
       </c>
       <c r="D1689" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1689" s="5">
+        <v>13</v>
+      </c>
+      <c r="E1689">
         <v>1</v>
       </c>
       <c r="F1689" t="s">
         <v>23</v>
       </c>
       <c r="G1689" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1689" s="4">
-        <v>44327</v>
+        <v>44322</v>
+      </c>
+      <c r="I1689" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="1690" spans="1:9" x14ac:dyDescent="0.25">
@@ -49916,39 +49949,42 @@
         <v>2</v>
       </c>
       <c r="B1690" s="5" t="s">
-        <v>787</v>
+        <v>649</v>
       </c>
       <c r="C1690" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D1690" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E1690" s="5">
         <v>1</v>
       </c>
-      <c r="F1690" t="s">
+      <c r="F1690" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G1690" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1690" s="4">
-        <v>44327</v>
+        <v>44322</v>
+      </c>
+      <c r="I1690" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1691" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1691" t="s">
+      <c r="A1691" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1691" s="5" t="s">
         <v>649</v>
       </c>
       <c r="C1691" t="s">
-        <v>758</v>
+        <v>784</v>
       </c>
       <c r="D1691" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1691" s="5">
         <v>1</v>
@@ -49956,83 +49992,77 @@
       <c r="F1691" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G1691" s="5" t="s">
-        <v>30</v>
+      <c r="G1691" t="s">
+        <v>31</v>
       </c>
       <c r="H1691" s="4">
-        <v>44327</v>
-      </c>
-      <c r="I1691" t="s">
-        <v>17</v>
+        <v>44323</v>
       </c>
     </row>
     <row r="1692" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1692" s="5" t="s">
+      <c r="A1692" t="s">
         <v>2</v>
       </c>
       <c r="B1692" s="5" t="s">
-        <v>787</v>
+        <v>624</v>
       </c>
       <c r="C1692" t="s">
-        <v>786</v>
+        <v>625</v>
       </c>
       <c r="D1692" t="s">
         <v>12</v>
       </c>
-      <c r="E1692" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1692" t="s">
+      <c r="E1692">
+        <v>1</v>
+      </c>
+      <c r="F1692" s="7" t="s">
         <v>23</v>
       </c>
       <c r="G1692" t="s">
         <v>31</v>
       </c>
       <c r="H1692" s="4">
-        <v>44327</v>
+        <v>44323</v>
       </c>
     </row>
     <row r="1693" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1693" t="s">
+      <c r="A1693" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1693" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="C1693" t="s">
-        <v>758</v>
+        <v>765</v>
+      </c>
+      <c r="C1693" s="5" t="s">
+        <v>757</v>
       </c>
       <c r="D1693" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="E1693" s="5">
         <v>1</v>
       </c>
       <c r="F1693" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1693" s="5" t="s">
-        <v>30</v>
+        <v>780</v>
+      </c>
+      <c r="G1693" t="s">
+        <v>31</v>
       </c>
       <c r="H1693" s="4">
-        <v>44327</v>
-      </c>
-      <c r="I1693" t="s">
-        <v>15</v>
+        <v>44320</v>
       </c>
     </row>
     <row r="1694" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1694" t="s">
+      <c r="A1694" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1694" s="5" t="s">
         <v>649</v>
       </c>
       <c r="C1694" t="s">
-        <v>758</v>
+        <v>784</v>
       </c>
       <c r="D1694" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E1694" s="5">
         <v>1</v>
@@ -50040,14 +50070,11 @@
       <c r="F1694" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G1694" s="5" t="s">
-        <v>30</v>
+      <c r="G1694" t="s">
+        <v>29</v>
       </c>
       <c r="H1694" s="4">
-        <v>44327</v>
-      </c>
-      <c r="I1694" t="s">
-        <v>15</v>
+        <v>44326</v>
       </c>
     </row>
     <row r="1695" spans="1:9" x14ac:dyDescent="0.25">
@@ -50055,28 +50082,25 @@
         <v>2</v>
       </c>
       <c r="B1695" s="5" t="s">
-        <v>765</v>
-      </c>
-      <c r="C1695" s="5" t="s">
-        <v>757</v>
+        <v>649</v>
+      </c>
+      <c r="C1695" t="s">
+        <v>784</v>
       </c>
       <c r="D1695" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1695" s="8" t="s">
-        <v>253</v>
+        <v>12</v>
+      </c>
+      <c r="E1695" s="5">
+        <v>1</v>
       </c>
       <c r="F1695" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G1695" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1695" s="4">
-        <v>44327</v>
-      </c>
-      <c r="I1695" t="s">
-        <v>17</v>
+        <v>44326</v>
       </c>
     </row>
     <row r="1696" spans="1:9" x14ac:dyDescent="0.25">
@@ -50084,28 +50108,25 @@
         <v>2</v>
       </c>
       <c r="B1696" s="5" t="s">
-        <v>765</v>
+        <v>749</v>
       </c>
       <c r="C1696" s="5" t="s">
-        <v>757</v>
+        <v>85</v>
       </c>
       <c r="D1696" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1696" s="8" t="s">
-        <v>254</v>
+        <v>666</v>
+      </c>
+      <c r="E1696" s="5">
+        <v>1</v>
       </c>
       <c r="F1696" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1696" t="s">
-        <v>30</v>
+        <v>783</v>
+      </c>
+      <c r="G1696" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="H1696" s="4">
-        <v>44327</v>
-      </c>
-      <c r="I1696" t="s">
-        <v>17</v>
+        <v>44326</v>
       </c>
     </row>
     <row r="1697" spans="1:9" x14ac:dyDescent="0.25">
@@ -50113,25 +50134,25 @@
         <v>2</v>
       </c>
       <c r="B1697" s="5" t="s">
-        <v>765</v>
+        <v>665</v>
       </c>
       <c r="C1697" s="5" t="s">
-        <v>757</v>
+        <v>85</v>
       </c>
       <c r="D1697" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="E1697" s="5">
         <v>1</v>
       </c>
       <c r="F1697" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1697" t="s">
-        <v>29</v>
+        <v>785</v>
+      </c>
+      <c r="G1697" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="H1697" s="4">
-        <v>44328</v>
+        <v>44326</v>
       </c>
     </row>
     <row r="1698" spans="1:9" x14ac:dyDescent="0.25">
@@ -50139,28 +50160,25 @@
         <v>2</v>
       </c>
       <c r="B1698" s="5" t="s">
-        <v>787</v>
-      </c>
-      <c r="C1698" t="s">
-        <v>786</v>
+        <v>765</v>
+      </c>
+      <c r="C1698" s="5" t="s">
+        <v>757</v>
       </c>
       <c r="D1698" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1698" s="5">
         <v>1</v>
       </c>
-      <c r="F1698" t="s">
-        <v>23</v>
+      <c r="F1698" s="5" t="s">
+        <v>781</v>
       </c>
       <c r="G1698" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1698" s="4">
-        <v>44328</v>
-      </c>
-      <c r="I1698" t="s">
-        <v>15</v>
+        <v>44320</v>
       </c>
     </row>
     <row r="1699" spans="1:9" x14ac:dyDescent="0.25">
@@ -50168,28 +50186,25 @@
         <v>2</v>
       </c>
       <c r="B1699" s="5" t="s">
-        <v>788</v>
+        <v>765</v>
       </c>
       <c r="C1699" s="5" t="s">
-        <v>85</v>
+        <v>757</v>
       </c>
       <c r="D1699" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="E1699" s="5">
         <v>1</v>
       </c>
-      <c r="F1699" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1699" s="5" t="s">
-        <v>30</v>
+      <c r="F1699" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="G1699" t="s">
+        <v>31</v>
       </c>
       <c r="H1699" s="4">
-        <v>44334</v>
-      </c>
-      <c r="I1699" t="s">
-        <v>15</v>
+        <v>44320</v>
       </c>
     </row>
     <row r="1700" spans="1:9" x14ac:dyDescent="0.25">
@@ -50197,265 +50212,286 @@
         <v>2</v>
       </c>
       <c r="B1700" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1700" s="5" t="s">
-        <v>85</v>
+        <v>612</v>
+      </c>
+      <c r="C1700" t="s">
+        <v>611</v>
       </c>
       <c r="D1700" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1700" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1700" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1700" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1700" s="4">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1701" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1701" t="s">
+        <v>793</v>
+      </c>
+      <c r="C1701" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1701" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1701">
+        <v>1</v>
+      </c>
+      <c r="F1701" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1701" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1701" s="4">
+        <v>44327</v>
+      </c>
+      <c r="I1701" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1702" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1702" t="s">
+        <v>793</v>
+      </c>
+      <c r="C1702" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1702" t="s">
         <v>44</v>
       </c>
-      <c r="E1700" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1700" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1700" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1700" s="4">
-        <v>44336</v>
-      </c>
-    </row>
-    <row r="1701" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1701" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1701" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1701" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1701" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1701" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1701" t="s">
-        <v>455</v>
-      </c>
-      <c r="G1701" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1701" s="4">
-        <v>44336</v>
-      </c>
-    </row>
-    <row r="1702" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1702" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1702" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1702" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1702" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1702" s="5">
+      <c r="E1702">
         <v>1</v>
       </c>
       <c r="F1702" t="s">
-        <v>284</v>
-      </c>
-      <c r="G1702" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="G1702" t="s">
+        <v>30</v>
       </c>
       <c r="H1702" s="4">
-        <v>44336</v>
+        <v>44327</v>
+      </c>
+      <c r="I1702" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="1703" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1703" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1703" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1703" s="5" t="s">
-        <v>85</v>
+      <c r="A1703" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1703" t="s">
+        <v>793</v>
+      </c>
+      <c r="C1703" t="s">
+        <v>268</v>
       </c>
       <c r="D1703" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1703" s="5">
+        <v>9</v>
+      </c>
+      <c r="E1703">
         <v>1</v>
       </c>
       <c r="F1703" t="s">
-        <v>461</v>
-      </c>
-      <c r="G1703" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="G1703" t="s">
+        <v>30</v>
       </c>
       <c r="H1703" s="4">
-        <v>44336</v>
+        <v>44327</v>
+      </c>
+      <c r="I1703" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="1704" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1704" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1704" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1704" s="5" t="s">
-        <v>85</v>
+      <c r="A1704" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1704" t="s">
+        <v>793</v>
+      </c>
+      <c r="C1704" t="s">
+        <v>268</v>
       </c>
       <c r="D1704" t="s">
         <v>66</v>
       </c>
-      <c r="E1704" s="5">
+      <c r="E1704">
         <v>1</v>
       </c>
       <c r="F1704" t="s">
         <v>23</v>
       </c>
-      <c r="G1704" s="5" t="s">
-        <v>31</v>
+      <c r="G1704" t="s">
+        <v>30</v>
       </c>
       <c r="H1704" s="4">
-        <v>44335</v>
+        <v>44327</v>
+      </c>
+      <c r="I1704" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="1705" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1705" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1705" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1705" s="5" t="s">
-        <v>85</v>
+      <c r="A1705" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1705" t="s">
+        <v>793</v>
+      </c>
+      <c r="C1705" t="s">
+        <v>268</v>
       </c>
       <c r="D1705" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1705">
+        <v>1</v>
+      </c>
+      <c r="F1705" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1705" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1705" s="4">
+        <v>44327</v>
+      </c>
+      <c r="I1705" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1706" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1706" t="s">
+        <v>793</v>
+      </c>
+      <c r="C1706" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1706" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1706">
+        <v>1</v>
+      </c>
+      <c r="F1706" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1706" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1706" s="4">
+        <v>44327</v>
+      </c>
+      <c r="I1706" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1707" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1707" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C1707" t="s">
+        <v>758</v>
+      </c>
+      <c r="D1707" t="s">
         <v>10</v>
       </c>
-      <c r="E1705" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1705" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1705" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1705" s="4">
-        <v>44335</v>
-      </c>
-      <c r="I1705" t="s">
+      <c r="E1707" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1707" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1707" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1707" s="4">
+        <v>44327</v>
+      </c>
+      <c r="I1707" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="1706" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1706" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1706" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1706" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1706" t="s">
+    <row r="1708" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1708" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1708" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C1708" t="s">
+        <v>758</v>
+      </c>
+      <c r="D1708" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1708" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1708" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1708" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1708" s="4">
+        <v>44327</v>
+      </c>
+      <c r="I1708" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1709" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1709" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C1709" t="s">
+        <v>758</v>
+      </c>
+      <c r="D1709" t="s">
         <v>59</v>
       </c>
-      <c r="E1706" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1706" t="s">
-        <v>789</v>
-      </c>
-      <c r="G1706" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1706" s="4">
-        <v>44335</v>
-      </c>
-      <c r="I1706" t="s">
+      <c r="E1709" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1709" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1709" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1709" s="4">
+        <v>44327</v>
+      </c>
+      <c r="I1709" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="1707" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1707" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1707" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1707" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1707" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1707" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1707" t="s">
-        <v>789</v>
-      </c>
-      <c r="G1707" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1707" s="4">
-        <v>44335</v>
-      </c>
-    </row>
-    <row r="1708" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1708" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1708" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1708" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1708" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1708" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1708" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1708" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1708" s="4">
-        <v>44335</v>
-      </c>
-    </row>
-    <row r="1709" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1709" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1709" s="5" t="s">
-        <v>788</v>
-      </c>
-      <c r="C1709" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1709" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1709" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1709" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1709" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1709" s="4">
-        <v>44335</v>
       </c>
     </row>
     <row r="1710" spans="1:9" x14ac:dyDescent="0.25">
@@ -50463,25 +50499,25 @@
         <v>2</v>
       </c>
       <c r="B1710" s="5" t="s">
-        <v>581</v>
+        <v>765</v>
       </c>
       <c r="C1710" s="5" t="s">
-        <v>85</v>
+        <v>757</v>
       </c>
       <c r="D1710" t="s">
-        <v>666</v>
+        <v>40</v>
       </c>
       <c r="E1710" s="5">
         <v>1</v>
       </c>
-      <c r="F1710" s="7" t="s">
-        <v>720</v>
+      <c r="F1710" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G1710" t="s">
         <v>31</v>
       </c>
       <c r="H1710" s="4">
-        <v>44334</v>
+        <v>44313</v>
       </c>
     </row>
     <row r="1711" spans="1:9" x14ac:dyDescent="0.25">
@@ -50489,25 +50525,28 @@
         <v>2</v>
       </c>
       <c r="B1711" s="5" t="s">
-        <v>788</v>
+        <v>765</v>
       </c>
       <c r="C1711" s="5" t="s">
-        <v>85</v>
+        <v>757</v>
       </c>
       <c r="D1711" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="E1711" s="5">
         <v>1</v>
       </c>
-      <c r="F1711" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1711" s="5" t="s">
-        <v>29</v>
+      <c r="F1711" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1711" t="s">
+        <v>30</v>
       </c>
       <c r="H1711" s="4">
-        <v>44335</v>
+        <v>44322</v>
+      </c>
+      <c r="I1711" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1712" spans="1:9" x14ac:dyDescent="0.25">
@@ -50515,80 +50554,77 @@
         <v>2</v>
       </c>
       <c r="B1712" s="5" t="s">
-        <v>665</v>
+        <v>765</v>
       </c>
       <c r="C1712" s="5" t="s">
-        <v>85</v>
+        <v>757</v>
       </c>
       <c r="D1712" t="s">
-        <v>667</v>
+        <v>45</v>
       </c>
       <c r="E1712" s="5">
         <v>1</v>
       </c>
-      <c r="F1712" s="7" t="s">
-        <v>790</v>
+      <c r="F1712" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="G1712" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1712" s="4">
-        <v>44337</v>
-      </c>
-      <c r="I1712" t="s">
-        <v>15</v>
+        <v>44326</v>
       </c>
     </row>
     <row r="1713" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1713" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1713" s="5" t="s">
-        <v>665</v>
-      </c>
-      <c r="C1713" s="5" t="s">
-        <v>85</v>
+      <c r="A1713" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1713" t="s">
+        <v>442</v>
       </c>
       <c r="D1713" t="s">
-        <v>667</v>
-      </c>
-      <c r="E1713" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1713" s="7" t="s">
-        <v>790</v>
+        <v>70</v>
+      </c>
+      <c r="E1713">
+        <v>2</v>
+      </c>
+      <c r="F1713" t="s">
+        <v>23</v>
       </c>
       <c r="G1713" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H1713" s="4">
-        <v>44337</v>
+        <v>44328</v>
       </c>
     </row>
     <row r="1714" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1714" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1714" s="5" t="s">
-        <v>791</v>
-      </c>
-      <c r="C1714" s="5" t="s">
-        <v>91</v>
+      <c r="A1714" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1714" t="s">
+        <v>442</v>
       </c>
       <c r="D1714" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1714" s="5">
+        <v>60</v>
+      </c>
+      <c r="E1714">
         <v>1</v>
       </c>
       <c r="F1714" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1714" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="G1714" t="s">
         <v>31</v>
       </c>
       <c r="H1714" s="4">
-        <v>44337</v>
+        <v>44328</v>
       </c>
     </row>
     <row r="1715" spans="1:9" x14ac:dyDescent="0.25">
@@ -50596,80 +50632,80 @@
         <v>2</v>
       </c>
       <c r="B1715" s="5" t="s">
-        <v>791</v>
+        <v>765</v>
       </c>
       <c r="C1715" s="5" t="s">
-        <v>91</v>
+        <v>757</v>
       </c>
       <c r="D1715" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1715" s="5">
         <v>1</v>
       </c>
-      <c r="F1715" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1715" s="5" t="s">
-        <v>31</v>
+      <c r="F1715" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1715" t="s">
+        <v>30</v>
       </c>
       <c r="H1715" s="4">
-        <v>44337</v>
+        <v>44348</v>
+      </c>
+      <c r="I1715" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1716" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1716" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1716" s="5" t="s">
-        <v>791</v>
-      </c>
-      <c r="C1716" s="5" t="s">
-        <v>91</v>
+      <c r="A1716" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>442</v>
       </c>
       <c r="D1716" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1716" s="5">
+        <v>64</v>
+      </c>
+      <c r="E1716">
         <v>1</v>
       </c>
       <c r="F1716" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1716" s="5" t="s">
-        <v>30</v>
+        <v>532</v>
+      </c>
+      <c r="G1716" t="s">
+        <v>31</v>
       </c>
       <c r="H1716" s="4">
-        <v>44342</v>
-      </c>
-      <c r="I1716" t="s">
-        <v>15</v>
+        <v>44330</v>
       </c>
     </row>
     <row r="1717" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1717" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1717" s="5" t="s">
-        <v>791</v>
-      </c>
-      <c r="C1717" s="5" t="s">
-        <v>91</v>
+      <c r="A1717" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>726</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>88</v>
       </c>
       <c r="D1717" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1717" s="5">
+        <v>62</v>
+      </c>
+      <c r="E1717">
         <v>1</v>
       </c>
       <c r="F1717" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1717" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="G1717" t="s">
         <v>31</v>
       </c>
       <c r="H1717" s="4">
-        <v>44343</v>
+        <v>44333</v>
       </c>
     </row>
     <row r="1718" spans="1:9" x14ac:dyDescent="0.25">
@@ -50677,25 +50713,25 @@
         <v>2</v>
       </c>
       <c r="B1718" s="5" t="s">
-        <v>791</v>
+        <v>581</v>
       </c>
       <c r="C1718" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D1718" t="s">
-        <v>42</v>
+        <v>666</v>
       </c>
       <c r="E1718" s="5">
         <v>1</v>
       </c>
-      <c r="F1718" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1718" s="5" t="s">
+      <c r="F1718" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="G1718" t="s">
         <v>31</v>
       </c>
       <c r="H1718" s="4">
-        <v>44343</v>
+        <v>44334</v>
       </c>
     </row>
     <row r="1719" spans="1:9" x14ac:dyDescent="0.25">
@@ -50703,13 +50739,13 @@
         <v>2</v>
       </c>
       <c r="B1719" s="5" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C1719" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D1719" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="E1719" s="5">
         <v>1</v>
@@ -50721,39 +50757,39 @@
         <v>30</v>
       </c>
       <c r="H1719" s="4">
-        <v>44342</v>
+        <v>44334</v>
       </c>
       <c r="I1719" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="1720" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1720" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1720" s="5" t="s">
-        <v>791</v>
-      </c>
-      <c r="C1720" s="5" t="s">
-        <v>91</v>
+      <c r="A1720" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>770</v>
       </c>
       <c r="D1720" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1720" s="5">
+        <v>666</v>
+      </c>
+      <c r="E1720">
         <v>1</v>
       </c>
       <c r="F1720" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1720" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="G1720" t="s">
         <v>30</v>
       </c>
       <c r="H1720" s="4">
-        <v>44342</v>
+        <v>44335</v>
       </c>
       <c r="I1720" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="1721" spans="1:9" x14ac:dyDescent="0.25">
@@ -50761,13 +50797,13 @@
         <v>2</v>
       </c>
       <c r="B1721" s="5" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C1721" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D1721" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E1721" s="5">
         <v>1</v>
@@ -50776,13 +50812,10 @@
         <v>23</v>
       </c>
       <c r="G1721" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1721" s="4">
-        <v>44342</v>
-      </c>
-      <c r="I1721" t="s">
-        <v>15</v>
+        <v>44335</v>
       </c>
     </row>
     <row r="1722" spans="1:9" x14ac:dyDescent="0.25">
@@ -50790,13 +50823,13 @@
         <v>2</v>
       </c>
       <c r="B1722" s="5" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C1722" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D1722" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E1722" s="5">
         <v>1</v>
@@ -50808,7 +50841,7 @@
         <v>30</v>
       </c>
       <c r="H1722" s="4">
-        <v>44342</v>
+        <v>44335</v>
       </c>
       <c r="I1722" t="s">
         <v>15</v>
@@ -50819,13 +50852,13 @@
         <v>2</v>
       </c>
       <c r="B1723" s="5" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C1723" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D1723" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E1723" s="5">
         <v>1</v>
@@ -50834,13 +50867,10 @@
         <v>23</v>
       </c>
       <c r="G1723" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1723" s="4">
-        <v>44342</v>
-      </c>
-      <c r="I1723" t="s">
-        <v>15</v>
+        <v>44335</v>
       </c>
     </row>
     <row r="1724" spans="1:9" x14ac:dyDescent="0.25">
@@ -50848,13 +50878,13 @@
         <v>2</v>
       </c>
       <c r="B1724" s="5" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C1724" s="5" t="s">
-        <v>786</v>
+        <v>85</v>
       </c>
       <c r="D1724" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E1724" s="5">
         <v>1</v>
@@ -50866,7 +50896,7 @@
         <v>31</v>
       </c>
       <c r="H1724" s="4">
-        <v>44343</v>
+        <v>44335</v>
       </c>
     </row>
     <row r="1725" spans="1:9" x14ac:dyDescent="0.25">
@@ -50874,25 +50904,28 @@
         <v>2</v>
       </c>
       <c r="B1725" s="5" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C1725" s="5" t="s">
-        <v>786</v>
+        <v>85</v>
       </c>
       <c r="D1725" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="E1725" s="5">
         <v>1</v>
       </c>
       <c r="F1725" t="s">
-        <v>23</v>
+        <v>789</v>
       </c>
       <c r="G1725" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1725" s="4">
-        <v>44343</v>
+        <v>44335</v>
+      </c>
+      <c r="I1725" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1726" spans="1:9" x14ac:dyDescent="0.25">
@@ -50900,25 +50933,25 @@
         <v>2</v>
       </c>
       <c r="B1726" s="5" t="s">
-        <v>649</v>
+        <v>788</v>
       </c>
       <c r="C1726" s="5" t="s">
-        <v>784</v>
+        <v>85</v>
       </c>
       <c r="D1726" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E1726" s="5">
         <v>1</v>
       </c>
       <c r="F1726" t="s">
-        <v>23</v>
+        <v>789</v>
       </c>
       <c r="G1726" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1726" s="4">
-        <v>44343</v>
+        <v>44335</v>
       </c>
     </row>
     <row r="1727" spans="1:9" x14ac:dyDescent="0.25">
@@ -50932,108 +50965,1324 @@
         <v>85</v>
       </c>
       <c r="D1727" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1727" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1727" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1727" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1727" s="4">
+        <v>44335</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1728" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1728" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1728">
+        <v>1</v>
+      </c>
+      <c r="F1728" t="s">
+        <v>795</v>
+      </c>
+      <c r="G1728" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1728" s="4">
+        <v>44335</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1729" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1729" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1729">
+        <v>3</v>
+      </c>
+      <c r="F1729" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1729" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1729" s="4">
+        <v>44335</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1730" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1730" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1730">
+        <v>1</v>
+      </c>
+      <c r="F1730" t="s">
+        <v>477</v>
+      </c>
+      <c r="G1730" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1730" s="4">
+        <v>44335</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1731" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>442</v>
+      </c>
+      <c r="D1731" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1731">
+        <v>1</v>
+      </c>
+      <c r="F1731" t="s">
+        <v>775</v>
+      </c>
+      <c r="G1731" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1731" s="4">
+        <v>44335</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1732" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1732" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="C1732" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1732" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1732" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1732" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1732" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1732" s="4">
+        <v>44336</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1733" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1733" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="C1733" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1733" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1733" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1733" t="s">
+        <v>455</v>
+      </c>
+      <c r="G1733" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1733" s="4">
+        <v>44336</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1734" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1734" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="C1734" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1734" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1734" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1734" t="s">
+        <v>284</v>
+      </c>
+      <c r="G1734" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1734" s="4">
+        <v>44336</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1735" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1735" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="C1735" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1735" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1735" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1735" t="s">
+        <v>461</v>
+      </c>
+      <c r="G1735" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1735" s="4">
+        <v>44336</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1736" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1736" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C1736" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1736" t="s">
+        <v>667</v>
+      </c>
+      <c r="E1736" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1736" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="G1736" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1736" s="4">
+        <v>44337</v>
+      </c>
+      <c r="I1736" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1737" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1737" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C1737" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1737" t="s">
+        <v>667</v>
+      </c>
+      <c r="E1737" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1737" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="G1737" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1737" s="4">
+        <v>44337</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1738" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1738" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1738" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="D1738" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1738" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1738" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1738" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1738" s="4">
+        <v>44343</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1739" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1739" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1739" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="D1739" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1739" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1739" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1739" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1739" s="4">
+        <v>44343</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1740" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1740" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1740">
+        <v>1</v>
+      </c>
+      <c r="F1740" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1740" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1740" s="4">
+        <v>44342</v>
+      </c>
+      <c r="I1740" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1741" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>745</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1741" t="s">
+        <v>667</v>
+      </c>
+      <c r="E1741">
+        <v>1</v>
+      </c>
+      <c r="F1741" t="s">
+        <v>796</v>
+      </c>
+      <c r="G1741" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1741" s="4">
+        <v>44342</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1742" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1742" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>786</v>
+      </c>
+      <c r="D1742" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1742" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1742" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1742" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1742" s="4">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1743" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1743" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>786</v>
+      </c>
+      <c r="D1743" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1743" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1743" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1743" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1743" s="4">
+        <v>44327</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1744" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1744" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1744" t="s">
+        <v>786</v>
+      </c>
+      <c r="D1744" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1744" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1744" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1744" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1744" s="4">
+        <v>44328</v>
+      </c>
+      <c r="I1744" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1745" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1745" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1745" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1745" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1745" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1745" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1745" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1745" s="4">
+        <v>44343</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1746" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1746" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1746" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1746" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1746" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1746" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1746" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1746" s="4">
+        <v>44343</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1747" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1747" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1747" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1747" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1747" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1747" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1747" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1747" s="4">
+        <v>44342</v>
+      </c>
+      <c r="I1747" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1748" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>793</v>
+      </c>
+      <c r="C1748" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1748" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1748">
+        <v>1</v>
+      </c>
+      <c r="F1748" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1748" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1748" s="4">
+        <v>44343</v>
+      </c>
+      <c r="I1748" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1749" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1749" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C1749" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="D1749" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1749" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1749" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1749" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1749" s="4">
+        <v>44343</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1750" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1750" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="C1750" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="D1750" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1750" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1750" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1750" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1750" s="4">
+        <v>44343</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1751" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1751" t="s">
+        <v>745</v>
+      </c>
+      <c r="C1751" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1751" t="s">
+        <v>666</v>
+      </c>
+      <c r="E1751">
+        <v>1</v>
+      </c>
+      <c r="F1751" t="s">
+        <v>796</v>
+      </c>
+      <c r="G1751" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1751" s="4">
+        <v>44343</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1752" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1752" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="C1752" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1752" t="s">
         <v>56</v>
       </c>
-      <c r="E1727" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1727" t="s">
+      <c r="E1752" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1752" t="s">
         <v>468</v>
       </c>
-      <c r="G1727" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1727" s="4">
+      <c r="G1752" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1752" s="4">
         <v>44343</v>
       </c>
     </row>
-    <row r="1728" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1728" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1728" s="5" t="s">
+    <row r="1753" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1753" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1753" s="5" t="s">
         <v>788</v>
       </c>
-      <c r="C1728" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1728" t="s">
+      <c r="C1753" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1753" t="s">
         <v>62</v>
       </c>
-      <c r="E1728" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1728" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1728" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1728" s="4">
+      <c r="E1753" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1753" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1753" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1753" s="4">
         <v>44343</v>
       </c>
     </row>
-    <row r="1729" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1729" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1729" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="C1729" s="5" t="s">
-        <v>784</v>
-      </c>
-      <c r="D1729" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1729" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1729" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1729" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1729" s="4">
-        <v>44343</v>
-      </c>
-    </row>
-    <row r="1730" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1730" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1730" s="5" t="s">
+    <row r="1754" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1754" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1754" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1754" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1754" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1754" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1754" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1754" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1754" s="4">
+        <v>44342</v>
+      </c>
+      <c r="I1754" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1755" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1755" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1755" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1755" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1755" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1755" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1755" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1755" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1756" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1756" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1756" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1756" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1756" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1756" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1756" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1756" s="4">
+        <v>44342</v>
+      </c>
+      <c r="I1756" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1757" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1757" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1757" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1757" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1757" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1757" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1757" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1757" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1758" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1758" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1758" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1758" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1758" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1758" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1758" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1758" s="4">
+        <v>44342</v>
+      </c>
+      <c r="I1758" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1759" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1759" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1759" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1759" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1759">
+        <v>1</v>
+      </c>
+      <c r="F1759" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1759" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1759" s="4">
+        <v>44347</v>
+      </c>
+      <c r="I1759" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1760" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1760" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1760" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1760" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1760" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1760" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1760" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1760" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1761" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1761" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1761" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1761" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1761" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1761" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1761" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1761" s="4">
+        <v>44337</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1762" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1762" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1762" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1762" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1762" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1762" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1762" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1762" s="4">
+        <v>44337</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1763" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1763" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1763" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1763" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1763" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1763" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1763" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1763" s="4">
+        <v>44342</v>
+      </c>
+      <c r="I1763" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1764" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1764" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1764" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1764" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1764" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1764" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1764" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1764" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1765" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1765" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1765" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1765" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1765" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1765" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1765" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1765" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1766" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1766" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C1766" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1766" t="s">
+        <v>667</v>
+      </c>
+      <c r="E1766" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1766" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="G1766" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1766" s="4">
+        <v>44347</v>
+      </c>
+      <c r="I1766" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1767" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1767" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C1767" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1767" t="s">
+        <v>667</v>
+      </c>
+      <c r="E1767" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1767" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="G1767" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1767" s="4">
+        <v>44347</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1768" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1768" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1768" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1768" t="s">
+        <v>667</v>
+      </c>
+      <c r="E1768" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1768" t="s">
+        <v>797</v>
+      </c>
+      <c r="G1768" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1768" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1769" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1769" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1769" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1769" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1769" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1769" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1769" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1769" s="4">
+        <v>44342</v>
+      </c>
+      <c r="I1769" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1770" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1770" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="C1770" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1770" t="s">
+        <v>666</v>
+      </c>
+      <c r="E1770" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1770" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="G1770" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1770" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1771" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1771" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1771" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1771" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1771" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1771" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1771" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1771" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1772" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1772" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1772" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1772" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1772" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1772" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1772" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1772" s="4">
+        <v>44349</v>
+      </c>
+      <c r="I1772" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1773" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1773" s="5" t="s">
         <v>765</v>
       </c>
-      <c r="C1730" s="5" t="s">
+      <c r="C1773" s="5" t="s">
         <v>757</v>
       </c>
-      <c r="D1730" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1730" s="5">
-        <v>1</v>
-      </c>
-      <c r="F1730" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1730" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1730" s="4">
-        <v>44344</v>
-      </c>
-      <c r="I1730" t="s">
-        <v>17</v>
+      <c r="D1773" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1773" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1773" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1773" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1773" s="4">
+        <v>44349</v>
+      </c>
+      <c r="I1773" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1774" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1774" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1774" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="D1774" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1774" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1774" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1774" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1774" s="4">
+        <v>44349</v>
+      </c>
+      <c r="I1774" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1775" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1775" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1775" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1775" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1775" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1775" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1775" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1775" s="4">
+        <v>44349</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1710" xr:uid="{666A33B2-D072-48D0-88E3-92275EF5620C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J1652">
-    <sortCondition ref="H2:H1652"/>
-    <sortCondition ref="C2:C1652"/>
-    <sortCondition ref="D2:D1652"/>
+  <autoFilter ref="A1:J1775" xr:uid="{666A33B2-D072-48D0-88E3-92275EF5620C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1602:J1771">
+      <sortCondition ref="C1:C1771"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J1759">
+    <sortCondition ref="H2:H1759"/>
+    <sortCondition ref="C2:C1759"/>
+    <sortCondition ref="D2:D1759"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update due to conversion of manual preprocess to the use of Power Automation.
</commit_message>
<xml_diff>
--- a/data/Wiesbaden First Pass Acceptance.xlsx
+++ b/data/Wiesbaden First Pass Acceptance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3C69DD-3840-4C08-A80D-12F05FBD0DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4D1356-7694-4D59-985D-540619A8858B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="105" yWindow="0" windowWidth="18000" windowHeight="12735" activeTab="1" xr2:uid="{203EF309-F09C-46D6-B42C-975B3263EA61}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="FPA" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FPA!$A$1:$J$1988</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FPA!$A$1:$J$1999</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12993" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13034" uniqueCount="889">
   <si>
     <t>SQA</t>
   </si>
@@ -2699,6 +2699,9 @@
   </si>
   <si>
     <t>GLT</t>
+  </si>
+  <si>
+    <t>PD-005425 Scan Barcode - TP2 - 2D Barcode Tests</t>
   </si>
 </sst>
 </file>
@@ -3581,11 +3584,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D811D2-7FE2-4400-8864-3E57D05FCB66}">
-  <dimension ref="A1:J1993"/>
+  <dimension ref="A1:J1999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1964" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1994" sqref="F1994"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1963" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2000" sqref="A2000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58130,7 +58133,7 @@
         <v>44382</v>
       </c>
     </row>
-    <row r="1985" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1985" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1985" s="5" t="s">
         <v>2</v>
       </c>
@@ -58156,7 +58159,7 @@
         <v>44382</v>
       </c>
     </row>
-    <row r="1986" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1986" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1986" s="5" t="s">
         <v>2</v>
       </c>
@@ -58182,7 +58185,7 @@
         <v>44382</v>
       </c>
     </row>
-    <row r="1987" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1987" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1987" s="5" t="s">
         <v>2</v>
       </c>
@@ -58208,7 +58211,7 @@
         <v>44382</v>
       </c>
     </row>
-    <row r="1988" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1988" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1988" s="5" t="s">
         <v>2</v>
       </c>
@@ -58234,7 +58237,7 @@
         <v>44382</v>
       </c>
     </row>
-    <row r="1989" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1989" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1989" s="5" t="s">
         <v>2</v>
       </c>
@@ -58260,7 +58263,7 @@
         <v>44383</v>
       </c>
     </row>
-    <row r="1990" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1990" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1990" s="5" t="s">
         <v>2</v>
       </c>
@@ -58286,7 +58289,7 @@
         <v>44383</v>
       </c>
     </row>
-    <row r="1991" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1991" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1991" s="5" t="s">
         <v>2</v>
       </c>
@@ -58312,7 +58315,7 @@
         <v>44383</v>
       </c>
     </row>
-    <row r="1992" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1992" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1992" s="5" t="s">
         <v>2</v>
       </c>
@@ -58338,7 +58341,7 @@
         <v>44384</v>
       </c>
     </row>
-    <row r="1993" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1993" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1993" s="5" t="s">
         <v>2</v>
       </c>
@@ -58364,8 +58367,179 @@
         <v>44384</v>
       </c>
     </row>
+    <row r="1994" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1994" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1994" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="C1994" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1994" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1994" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1994" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1994" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1994" s="4">
+        <v>44385</v>
+      </c>
+      <c r="I1994" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1995" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1995" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="C1995" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1995" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1995" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1995" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1995" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1995" s="4">
+        <v>44385</v>
+      </c>
+      <c r="I1995" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1996" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1996" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1996" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="D1996" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1996" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1996" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1996" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1996" s="4">
+        <v>44386</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1997" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1997" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="C1997" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1997" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1997" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1997" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1997" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1997" s="4">
+        <v>44386</v>
+      </c>
+      <c r="I1997" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1998" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1998" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="C1998" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1998" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1998" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1998" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1998" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1998" s="4">
+        <v>44386</v>
+      </c>
+      <c r="I1998" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1999" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1999" s="5" t="s">
+        <v>883</v>
+      </c>
+      <c r="C1999" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1999" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1999" s="5">
+        <v>1</v>
+      </c>
+      <c r="F1999" t="s">
+        <v>888</v>
+      </c>
+      <c r="G1999" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1999" s="4">
+        <v>44386</v>
+      </c>
+      <c r="I1999" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J1988" xr:uid="{666A33B2-D072-48D0-88E3-92275EF5620C}">
+  <autoFilter ref="A1:J1999" xr:uid="{666A33B2-D072-48D0-88E3-92275EF5620C}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J1811">
       <sortCondition ref="H1:H1811"/>
     </sortState>

</xml_diff>